<commit_message>
Multiple edits and bug fixes
Replaces hard-coded (and sometimes in comments) reference to 2100 with variable.
Fixes NT future management bug (was tilling).
Removes extra N application in last corn year (and all future years).
Re-runs all models through 2100 and 2050.
</commit_message>
<xml_diff>
--- a/Data/LRF/Historical Land Use and Yields/TX-Lubbock County historical yields and C input.xlsx
+++ b/Data/LRF/Historical Land Use and Yields/TX-Lubbock County historical yields and C input.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\edmaas\Documents\Modeling\Data\LRF\Historical Land Use and Yields\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16CFE7EB-8299-43A4-AABA-F491568C2F68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13569CDB-9C13-4E20-83B7-728E6E91C14D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29940" yWindow="1140" windowWidth="22575" windowHeight="14205" activeTab="1" xr2:uid="{3345FC2A-340F-4F21-8A3A-F9BB132E4BBF}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{3345FC2A-340F-4F21-8A3A-F9BB132E4BBF}"/>
   </bookViews>
   <sheets>
     <sheet name="Census Data" sheetId="1" r:id="rId1"/>
@@ -253,22 +253,22 @@
   <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -706,16 +706,16 @@
       <c r="Y1" t="s">
         <v>21</v>
       </c>
-      <c r="AA1" s="6" t="s">
+      <c r="AA1" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="AB1" s="6"/>
-      <c r="AC1" s="6"/>
-      <c r="AE1" s="7" t="s">
+      <c r="AB1" s="4"/>
+      <c r="AC1" s="4"/>
+      <c r="AE1" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="AF1" s="7"/>
-      <c r="AG1" s="7"/>
+      <c r="AF1" s="3"/>
+      <c r="AG1" s="3"/>
     </row>
     <row r="2" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A2">
@@ -2564,13 +2564,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B3F8D8B-0477-42CC-AB22-6EF0A0651159}">
-  <dimension ref="A1:F85"/>
+  <dimension ref="A1:F88"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B24" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B78" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F41" sqref="F41"/>
+      <selection pane="bottomRight" activeCell="E89" sqref="E89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2584,15 +2584,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="C1" s="5"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="2" t="s">
+      <c r="C1" s="6"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="F1" s="3"/>
+      <c r="F1" s="7"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
@@ -2604,7 +2604,7 @@
       <c r="C2" t="s">
         <v>26</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="2" t="s">
         <v>24</v>
       </c>
       <c r="E2" t="s">
@@ -2676,7 +2676,7 @@
         <v>21.441532984534671</v>
       </c>
       <c r="E8">
-        <f t="shared" ref="E4:E67" si="0">B8*56*453.592/4046.86</f>
+        <f t="shared" ref="E8:E23" si="0">B8*56*453.592/4046.86</f>
         <v>4.2273401521113865</v>
       </c>
       <c r="F8">
@@ -2876,7 +2876,7 @@
         <v>38.2371428571428</v>
       </c>
       <c r="E36">
-        <f t="shared" ref="E36:E85" si="1">C36*453.592/4046.86</f>
+        <f t="shared" ref="E36:E82" si="1">C36*453.592/4046.86</f>
         <v>46.338465679928724</v>
       </c>
       <c r="F36">
@@ -3792,7 +3792,7 @@
         <v>70.960637944660078</v>
       </c>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A81" s="1">
         <v>2017</v>
       </c>
@@ -3809,7 +3809,7 @@
         <v>55.150604007386775</v>
       </c>
     </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A82" s="1">
         <v>2018</v>
       </c>
@@ -3822,19 +3822,39 @@
         <v>34.203234876616229</v>
       </c>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A83" s="1">
         <v>2019</v>
       </c>
     </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A84" s="1">
         <v>2020</v>
       </c>
     </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A85" s="1">
         <v>2021</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="E87">
+        <f>AVERAGE(E64:E77)</f>
+        <v>46.28488827870769</v>
+      </c>
+      <c r="F87">
+        <f>AVERAGE(F64:F77)</f>
+        <v>196.54246098645766</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="E88">
+        <f>AVERAGE(E36:E77)</f>
+        <v>38.632651140594589</v>
+      </c>
+      <c r="F88">
+        <f>AVERAGE(F36:F77)</f>
+        <v>207.16331774793284</v>
       </c>
     </row>
   </sheetData>

</xml_diff>